<commit_message>
Added more explored data sets
Expanded the list of explored data sets. Bookkeeping excel file updated.
</commit_message>
<xml_diff>
--- a/List of data sets.xlsx
+++ b/List of data sets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varun\Documents\GitHub\Obstacle-avoiding-agents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B71862-8EA2-4FD5-8026-C7F779ABA796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEA192D-8978-4059-9219-39B6942D0CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Name</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Continuous model sweep_expt</t>
+  </si>
+  <si>
+    <t>Data10</t>
+  </si>
+  <si>
+    <t>Noise  + numNeighbours</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,6 +626,17 @@
         <v>20210202</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>20220408</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>